<commit_message>
xlsx -> csv works
</commit_message>
<xml_diff>
--- a/tests/files/ts_xlsx/conversionIn.xlsx
+++ b/tests/files/ts_xlsx/conversionIn.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t xml:space="preserve">context</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">../../QML/OggettiEditDash/AddNewForm.qml - 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../../QML/OggettiEditDash/AddNewForm.qml – 21</t>
   </si>
   <si>
     <t xml:space="preserve">2.1</t>
@@ -65,7 +68,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -85,6 +88,11 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="0"/>
     </font>
     <font>
@@ -136,7 +144,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -149,7 +157,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -173,7 +185,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -184,7 +196,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -220,15 +232,18 @@
       <c r="D2" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="F2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="3"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>